<commit_message>
feat: add multiple fibonacci implementations with test runs and experiment config
</commit_message>
<xml_diff>
--- a/outputs/results.xlsx
+++ b/outputs/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2045,6 +2045,1579 @@
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>fibonacci_2-1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:34.768048</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_sequence = fibonacci_2(n - 1)
+        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
+        return fib_sequence
+```</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_sequence = fibonacci_2(n - 1)
+        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
+        return fib_sequence
+</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>fibonacci_2-2</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:36.928516</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>fibonacci_2-3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:38.100756</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fibonacci_2-4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:39.674075</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>fibonacci_2-5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:41.235849</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>5</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n-1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n-1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>fibonacci_3-1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:43.290280</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = []
+    a, b = 0, 1
+    for _ in range(n):
+        fib_list.append(a)
+        a, b = b, a + b
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = []
+    a, b = 0, 1
+    for _ in range(n):
+        fib_list.append(a)
+        a, b = b, a + b
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>fibonacci_3-2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:44.334586</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fibonacci_list = [0, 1, 1]
+    for i in range(3, n):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fibonacci_list = [0, 1, 1]
+    for i in range(3, n):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>fibonacci_3-3</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:45.621324</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib_list = [0, 1]
+    for i in range(1, 2):
+        fib_list.append(fib_list[i] + fib_list[i-1])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib_list = [0, 1]
+    for i in range(1, 2):
+        fib_list.append(fib_list[i] + fib_list[i-1])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>fibonacci_3-4</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:47.508039</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>4</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    for i in range(3, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    for i in range(3, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>fibonacci_3-5</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:48.428784</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_sequence = [0, 1, 1]
+    for i in range(3, n):
+        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2] + fib_sequence[i-3])
+    return fib_sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_sequence = [0, 1, 1]
+    for i in range(3, n):
+        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2] + fib_sequence[i-3])
+    return fib_sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>fibonacci_4-1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:51.154855</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>fibonacci_4-2</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:52.042249</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>fibonacci_4-3</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:52.987756</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        next_num = fibonacci_list[i-1] + fibonacci_list[i-2]
+        fibonacci_list.append(next_num)
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        next_num = fibonacci_list[i-1] + fibonacci_list[i-2]
+        fibonacci_list.append(next_num)
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fibonacci_4-4</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:53.863779</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>4</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci = [0, 1]
+    for i in range(2, 4):
+        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci = [0, 1]
+    for i in range(2, 4):
+        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fibonacci_4-5</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:54.744816</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>fibonacci_5-1</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:55.997196</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_5(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+result = fibonacci_5(5)
+print(result)
+```</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 1:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_5(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+result = fibonacci_5(5)
+print(result)
+</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fibonacci_5-2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:57.443711</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]
+```</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]
+</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fibonacci_5-3</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:08:58.789255</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_5(n-1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_5(n-1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fibonacci_5-4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:00.678303</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>4</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_5(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+print(fibonacci_5(5))
+```</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_5(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+print(fibonacci_5(5))
+</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>fibonacci_5-5</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:01.730225</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>5</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]
+```</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]
+</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>fibonacci-1</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:03.169409</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fibonacci_list = [0, 1]
+    for i in range(2, n):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fibonacci_list = [0, 1]
+    for i in range(2, n):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>fibonacci-2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:04.131325</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    result = []
+    a, b = 0, 1
+    for _ in range(n):
+        result.append(a)
+        a, b = b, a + b
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    result = []
+    a, b = 0, 1
+    for _ in range(n):
+        result.append(a)
+        a, b = b, a + b
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>fibonacci-3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:05.134661</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>fibonacci-4</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:06.585064</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>4</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>fibonacci-5</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:09:07.803538</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>5</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add improved repeatability analysis with Excel reporting for fibonacci experiments
</commit_message>
<xml_diff>
--- a/outputs/results.xlsx
+++ b/outputs/results.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:49.117570</t>
+          <t>2025-07-30T16:24:04.511319</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,7 +543,7 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n - 1)
+        fib = fibonacci_2(n-1)
         fib.append(fib[-1] + fib[-2])
         return fib
 ```</t>
@@ -559,7 +559,7 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n - 1)
+        fib = fibonacci_2(n-1)
         fib.append(fib[-1] + fib[-2])
         return fib
 </t>
@@ -578,7 +578,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:52.429424</t>
+          <t>2025-07-30T16:24:06.090495</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:53.897991</t>
+          <t>2025-07-30T16:24:07.591182</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:55.466727</t>
+          <t>2025-07-30T16:24:08.748114</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -753,7 +753,7 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n - 1)
+        fib = fibonacci_2(n-1)
         fib.append(fib[-1] + fib[-2])
         return fib
 ```</t>
@@ -769,7 +769,7 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n - 1)
+        fib = fibonacci_2(n-1)
         fib.append(fib[-1] + fib[-2])
         return fib
 </t>
@@ -788,7 +788,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:56.706096</t>
+          <t>2025-07-30T16:24:10.647482</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:57.863007</t>
+          <t>2025-07-30T16:24:12.081006</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -888,8 +888,9 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        next_fib = fib_list[-1] + fib_list[-2] + fib_list[-3]
+        fib_list.append(next_fib)
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -899,8 +900,9 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        next_fib = fib_list[-1] + fib_list[-2] + fib_list[-3]
+        fib_list.append(next_fib)
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -917,7 +919,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:58.856077</t>
+          <t>2025-07-30T16:24:13.206306</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -947,8 +949,9 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        next_num = fib_list[-1] + fib_list[-2] + fib_list[-3]
+        fib_list.append(next_num)
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -958,8 +961,9 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        next_num = fib_list[-1] + fib_list[-2] + fib_list[-3]
+        fib_list.append(next_num)
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -976,7 +980,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-07-30T15:59:59.971336</t>
+          <t>2025-07-30T16:24:18.573785</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1006,8 +1010,8 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        fib_list.append(fib_list[-1] + fib_list[-2] + fib_list[-3])
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -1017,8 +1021,8 @@
 def fibonacci_3(n):
     fib_list = [0, 1, 1]
     for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+        fib_list.append(fib_list[-1] + fib_list[-2] + fib_list[-3])
+    return fib_list[:n]
 ```</t>
         </is>
       </c>
@@ -1035,7 +1039,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:00.889742</t>
+          <t>2025-07-30T16:24:19.918247</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1063,10 +1067,10 @@
         <is>
           <t>```python
 def fibonacci_3(n):
-    fib_list = [0, 1, 1]
-    for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+    fib_series = [0, 1]
+    for i in range(2, n):
+        fib_series.append(fib_series[i-1] + fib_series[i-2])
+    return fib_series
 ```</t>
         </is>
       </c>
@@ -1074,10 +1078,10 @@
         <is>
           <t>```python
 def fibonacci_3(n):
-    fib_list = [0, 1, 1]
-    for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+    fib_series = [0, 1]
+    for i in range(2, n):
+        fib_series.append(fib_series[i-1] + fib_series[i-2])
+    return fib_series
 ```</t>
         </is>
       </c>
@@ -1094,7 +1098,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:02.044615</t>
+          <t>2025-07-30T16:24:22.369699</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1121,10 +1125,12 @@
       <c r="H11" t="inlineStr">
         <is>
           <t>```python
-def fibonacci_3(n):
-    fib_list = [0, 1, 1]
-    for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
+def fibonacci_3():
+    n = 3
+    fib_list = [0, 1]
+    while n &gt; 0:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        n -= 1
     return fib_list
 ```</t>
         </is>
@@ -1132,10 +1138,12 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>```python
-def fibonacci_3(n):
-    fib_list = [0, 1, 1]
-    for i in range(3, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
+def fibonacci_3():
+    n = 3
+    fib_list = [0, 1]
+    while n &gt; 0:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        n -= 1
     return fib_list
 ```</t>
         </is>
@@ -1153,7 +1161,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:03.180758</t>
+          <t>2025-07-30T16:24:24.007813</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1181,10 +1189,10 @@
         <is>
           <t>```python
 def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+    fibonacci = [0, 1]
+    while len(fibonacci) &lt; 4:
+        fibonacci.append(fibonacci[-1] + fibonacci[-2])
+    return fibonacci
 ```</t>
         </is>
       </c>
@@ -1192,10 +1200,10 @@
         <is>
           <t>```python
 def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
+    fibonacci = [0, 1]
+    while len(fibonacci) &lt; 4:
+        fibonacci.append(fibonacci[-1] + fibonacci[-2])
+    return fibonacci
 ```</t>
         </is>
       </c>
@@ -1212,7 +1220,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:04.082362</t>
+          <t>2025-07-30T16:24:25.190798</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1237,183 +1245,6 @@
         </is>
       </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>fibonacci_4-3</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:05.053150</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>3</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>fibonacci_4-4</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:06.003406</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>fibonacci_4-5</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:06.911508</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_4():
@@ -1424,7 +1255,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_4():
@@ -1435,6 +1266,185 @@
 ```</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>fibonacci_4-3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:26.004580</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci = [0, 1]
+    for i in range(2, 4):
+        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci = [0, 1]
+    for i in range(2, 4):
+        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>fibonacci_4-4</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:27.065037</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    while len(fib_list) &lt; 4:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    while len(fib_list) &lt; 4:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>fibonacci_4-5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:28.126162</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    while len(fib_list) &lt; 4:
+        next_num = fib_list[-1] + fib_list[-2]
+        fib_list.append(next_num)
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    while len(fib_list) &lt; 4:
+        next_num = fib_list[-1] + fib_list[-2]
+        fib_list.append(next_num)
+    return fib_list
+```</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1448,7 +1458,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:08.772442</t>
+          <t>2025-07-30T16:24:29.064881</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1473,6 +1483,137 @@
         </is>
       </c>
       <c r="H17" t="inlineStr">
+        <is>
+          <t>def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2) if n &gt; 1 else 0
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2) if n &gt; 1 else 0
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>fibonacci_5-2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:30.234705</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_sequence = fibonacci_5(n - 1)
+        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
+        return fib_sequence
+print(fibonacci_5(5))
+```</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_sequence = fibonacci_5(n - 1)
+        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
+        return fib_sequence
+print(fibonacci_5(5))
+</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>fibonacci_5-3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:31.138333</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_5(n):
@@ -1485,7 +1626,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t xml:space="preserve">def fibonacci_5(n):
     if n &lt;= 1:
@@ -1497,44 +1638,44 @@
 </t>
         </is>
       </c>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>fibonacci_5-2</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:09.776234</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fibonacci_5-4</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:32.275774</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" t="inlineStr">
+      <c r="F20" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_5(n):
@@ -1547,7 +1688,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t xml:space="preserve">def fibonacci_5(n):
     if n &lt;= 1:
@@ -1559,44 +1700,44 @@
 </t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>fibonacci_5-3</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:11.699069</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>fibonacci_5-5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:33.682539</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>3</v>
-      </c>
-      <c r="G19" t="inlineStr">
+      <c r="F21" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_5(n):
@@ -1609,7 +1750,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t xml:space="preserve">def fibonacci_5(n):
     if n &lt;= 1:
@@ -1621,130 +1762,6 @@
 </t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>fibonacci_5-4</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:13.321364</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>4</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5_list():
-    return [fibonacci_5(i) for i in range(5)]
-```</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5():
-    return [fibonacci_5(i) for i in range(5)]
-</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>fibonacci_5-5</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:14.256607</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>5</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5_list():
-    return [fibonacci_5(i) for i in range(5)]
-```</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5():
-    return [fibonacci_5(i) for i in range(5)]
-</t>
-        </is>
-      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1758,7 +1775,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:15.753170</t>
+          <t>2025-07-30T16:24:36.776402</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1817,7 +1834,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:16.654662</t>
+          <t>2025-07-30T16:24:37.944457</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1876,7 +1893,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-07-30T16:00:17.683619</t>
+          <t>2025-07-30T16:24:39.127200</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1901,6 +1918,65 @@
         </is>
       </c>
       <c r="H24" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>fibonacci-4</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:40.300268</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
@@ -1911,7 +1987,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
@@ -1922,121 +1998,62 @@
 ```</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>fibonacci-4</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:19.095677</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fibonacci-5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:24:41.257984</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>4</v>
-      </c>
-      <c r="G25" t="inlineStr">
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
     fib_list = [0, 1]
     while len(fib_list) &lt; n:
         fib_list.append(fib_list[-1] + fib_list[-2])
-    return fib_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
     fib_list = [0, 1]
     while len(fib_list) &lt; n:
         fib_list.append(fib_list[-1] + fib_list[-2])
-    return fib_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>fibonacci-5</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:00:20.512820</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>5</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    fib_list = [0, 1]
-    while len(fib_list) &lt; n:
-        fib_list.append(fib_list[-1] + fib_list[-2])
-    return fib_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    fib_list = [0, 1]
-    while len(fib_list) &lt; n:
-        fib_list.append(fib_list[-1] + fib_list[-2])
-    return fib_list[:n]
+    return fib_list
 ```</t>
         </is>
       </c>
@@ -2053,7 +2070,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:34.768048</t>
+          <t>2025-07-30T16:29:12.271018</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2088,9 +2105,9 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib_sequence = fibonacci_2(n - 1)
-        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
-        return fib_sequence
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
 ```</t>
         </is>
       </c>
@@ -2104,9 +2121,9 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib_sequence = fibonacci_2(n - 1)
-        fib_sequence.append(fib_sequence[-1] + fib_sequence[-2])
-        return fib_sequence
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
 </t>
         </is>
       </c>
@@ -2123,7 +2140,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:36.928516</t>
+          <t>2025-07-30T16:29:13.529500</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2158,15 +2175,15 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib_list = fibonacci_2(n - 1)
-        fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
 ```</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_2(n):
+          <t>def fibonacci_2(n):
     if n &lt;= 0:
         return []
     elif n == 1:
@@ -2176,8 +2193,7 @@
     else:
         fib_list = fibonacci_2(n - 1)
         fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-</t>
+        return fib_list</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -2193,7 +2209,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:38.100756</t>
+          <t>2025-07-30T16:29:15.155985</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2236,7 +2252,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_2(n):
+          <t>def fibonacci_2(n):
     if n &lt;= 0:
         return []
     elif n == 1:
@@ -2244,10 +2260,9 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n - 1)
-        fib.append(fib[-1] + fib[-2])
-        return fib
-</t>
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
@@ -2263,7 +2278,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:39.674075</t>
+          <t>2025-07-30T16:29:16.318582</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2306,7 +2321,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_2(n):
+          <t>def fibonacci_2(n):
     if n &lt;= 0:
         return []
     elif n == 1:
@@ -2316,8 +2331,7 @@
     else:
         fib_list = fibonacci_2(n - 1)
         fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-</t>
+        return fib_list</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -2333,7 +2347,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:41.235849</t>
+          <t>2025-07-30T16:29:17.746489</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2368,15 +2382,15 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n-1)
-        fib.append(fib[-1] + fib[-2])
-        return fib
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
 ```</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_2(n):
+          <t>def fibonacci_2(n):
     if n &lt;= 0:
         return []
     elif n == 1:
@@ -2384,10 +2398,9 @@
     elif n == 2:
         return [0, 1]
     else:
-        fib = fibonacci_2(n-1)
-        fib.append(fib[-1] + fib[-2])
-        return fib
-</t>
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -2403,7 +2416,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:43.290280</t>
+          <t>2025-07-30T16:29:18.576939</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2428,6 +2441,65 @@
         </is>
       </c>
       <c r="H32" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fibonacci = [0, 1]
+    for i in range(1, 2):
+        fibonacci.append(fibonacci[i] + fibonacci[i-1])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fibonacci = [0, 1]
+    for i in range(1, 2):
+        fibonacci.append(fibonacci[i] + fibonacci[i-1])
+    return fibonacci
+```</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>fibonacci_3-2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:19.977503</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_3(n):
@@ -2440,7 +2512,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_3(n):
@@ -2453,65 +2525,6 @@
 ```</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>fibonacci_3-2</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:44.334586</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_3(n):
-    fibonacci_list = [0, 1, 1]
-    for i in range(3, n):
-        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
-    return fibonacci_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_3(n):
-    fibonacci_list = [0, 1, 1]
-    for i in range(3, n):
-        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
-    return fibonacci_list[:n]
-```</t>
-        </is>
-      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -2525,7 +2538,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:45.621324</t>
+          <t>2025-07-30T16:29:20.801147</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2552,22 +2565,22 @@
       <c r="H34" t="inlineStr">
         <is>
           <t>```python
-def fibonacci_3():
-    fib_list = [0, 1]
-    for i in range(1, 2):
-        fib_list.append(fib_list[i] + fib_list[i-1])
-    return fib_list
+def fibonacci_3(n):
+    fib = [0, 1, 1]
+    for i in range(3, n):
+        fib.append(fib[i-1] + fib[i-2] + fib[i-3])
+    return fib[:n]
 ```</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
           <t>```python
-def fibonacci_3():
-    fib_list = [0, 1]
-    for i in range(1, 2):
-        fib_list.append(fib_list[i] + fib_list[i-1])
-    return fib_list
+def fibonacci_3(n):
+    fib = [0, 1, 1]
+    for i in range(3, n):
+        fib.append(fib[i-1] + fib[i-2] + fib[i-3])
+    return fib[:n]
 ```</t>
         </is>
       </c>
@@ -2584,7 +2597,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:47.508039</t>
+          <t>2025-07-30T16:29:21.786668</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2609,6 +2622,65 @@
         </is>
       </c>
       <c r="H35" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fibonacci_numbers = [0, 1]
+    for i in range(2, n):
+        fibonacci_numbers.append(fibonacci_numbers[i-1] + fibonacci_numbers[i-2])
+    return fibonacci_numbers[:3]
+```</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fibonacci_numbers = [0, 1]
+    for i in range(2, n):
+        fibonacci_numbers.append(fibonacci_numbers[i-1] + fibonacci_numbers[i-2])
+    return fibonacci_numbers[:3]
+```</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>fibonacci_3-5</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:22.767575</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_3(n):
@@ -2619,7 +2691,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_3(n):
@@ -2630,65 +2702,6 @@
 ```</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>fibonacci_3-5</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:48.428784</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>5</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_3(n):
-    fib_sequence = [0, 1, 1]
-    for i in range(3, n):
-        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2] + fib_sequence[i-3])
-    return fib_sequence[:n]
-```</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_3(n):
-    fib_sequence = [0, 1, 1]
-    for i in range(3, n):
-        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2] + fib_sequence[i-3])
-    return fib_sequence[:n]
-```</t>
-        </is>
-      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2702,7 +2715,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:51.154855</t>
+          <t>2025-07-30T16:29:24.139960</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2761,7 +2774,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:52.042249</t>
+          <t>2025-07-30T16:29:25.544072</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2786,6 +2799,183 @@
         </is>
       </c>
       <c r="H38" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    result = [0, 1]
+    while len(result) &lt; 4:
+        result.append(result[-1] + result[-2])
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    result = [0, 1]
+    while len(result) &lt; 4:
+        result.append(result[-1] + result[-2])
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>fibonacci_4-3</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:29.071416</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    sequence = [0, 1]
+    while len(sequence) &lt; 4:
+        sequence.append(sequence[-1] + sequence[-2])
+    return sequence
+```</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    sequence = [0, 1]
+    while len(sequence) &lt; 4:
+        sequence.append(sequence[-1] + sequence[-2])
+    return sequence
+```</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fibonacci_4-4</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:29.959570</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>4</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fibonacci_4-5</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:31.763983</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_4():
@@ -2796,7 +2986,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_4():
@@ -2807,185 +2997,6 @@
 ```</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>fibonacci_4-3</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:52.987756</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>3</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fibonacci_list = [0, 1]
-    for i in range(2, 4):
-        next_num = fibonacci_list[i-1] + fibonacci_list[i-2]
-        fibonacci_list.append(next_num)
-    return fibonacci_list
-```</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fibonacci_list = [0, 1]
-    for i in range(2, 4):
-        next_num = fibonacci_list[i-1] + fibonacci_list[i-2]
-        fibonacci_list.append(next_num)
-    return fibonacci_list
-```</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>fibonacci_4-4</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:53.863779</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>4</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fibonacci = [0, 1]
-    for i in range(2, 4):
-        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
-    return fibonacci
-```</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fibonacci = [0, 1]
-    for i in range(2, 4):
-        fibonacci.append(fibonacci[i-1] + fibonacci[i-2])
-    return fibonacci
-```</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>fibonacci_4-5</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:54.744816</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>5</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_4():
-    fib_list = [0, 1]
-    for i in range(2, 4):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
-    return fib_list
-```</t>
-        </is>
-      </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2999,7 +3010,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-07-30T16:08:55.997196</t>
+          <t>2025-07-30T16:29:33.262665</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3024,134 +3035,6 @@
         </is>
       </c>
       <c r="H42" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_5(n):
-    if n &lt;= 1:
-        return [0, 1]
-    else:
-        fib_list = fibonacci_5(n - 1)
-        fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-result = fibonacci_5(5)
-print(result)
-```</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">def fibonacci_5(n):
-    if n &lt;= 1:
-        return [0, 1]
-    else:
-        fib_list = fibonacci_5(n - 1)
-        fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-result = fibonacci_5(5)
-print(result)
-</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>fibonacci_5-2</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:57.443711</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>2</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5_list():
-    return [fibonacci_5(i) for i in range(5)]
-```</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">def fibonacci_5(n):
-    if n &lt;= 1:
-        return n
-    else:
-        return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5():
-    return [fibonacci_5(i) for i in range(5)]
-</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>fibonacci_5-3</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:08:58.789255</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>3</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
         <is>
           <t>```python
 def fibonacci_5(n):
@@ -3168,7 +3051,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="I42" t="inlineStr">
         <is>
           <t xml:space="preserve">def fibonacci_5(n):
     if n &lt;= 0:
@@ -3184,6 +3067,144 @@
 </t>
         </is>
       </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fibonacci_5-2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:35.017393</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fibonacci_5-3</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:36.999283</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
+```</t>
+        </is>
+      </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -3197,7 +3218,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-07-30T16:09:00.678303</t>
+          <t>2025-07-30T16:29:39.052920</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3226,30 +3247,27 @@
           <t>```python
 def fibonacci_5(n):
     if n &lt;= 1:
-        return [0]
-    elif n == 2:
-        return [0, 1]
-    else:
-        fib_list = fibonacci_5(n - 1)
-        fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-print(fibonacci_5(5))
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    result = [fibonacci_5(i) for i in range(5)]
+    return result
 ```</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_5(n):
+          <t>```python
+def fibonacci_5(n):
     if n &lt;= 1:
-        return [0]
-    elif n == 2:
-        return [0, 1]
-    else:
-        fib_list = fibonacci_5(n - 1)
-        fib_list.append(fib_list[-1] + fib_list[-2])
-        return fib_list
-print(fibonacci_5(5))
-</t>
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    result = [fibonacci_5(i) for i in range(5)]
+    return result
+```</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -3265,7 +3283,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-07-30T16:09:01.730225</t>
+          <t>2025-07-30T16:29:40.886910</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3298,20 +3316,27 @@
     else:
         return fibonacci_5(n-1) + fibonacci_5(n-2)
 def fibonacci_5_list():
-    return [fibonacci_5(i) for i in range(5)]
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
 ```</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t xml:space="preserve">def fibonacci_5(n):
+          <t>```python
+def fibonacci_5(n):
     if n &lt;= 1:
         return n
     else:
         return fibonacci_5(n-1) + fibonacci_5(n-2)
-def fibonacci_5():
-    return [fibonacci_5(i) for i in range(5)]
-</t>
+def fibonacci_5_list():
+    fib_list = []
+    for i in range(5):
+        fib_list.append(fibonacci_5(i))
+    return fib_list
+```</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -3327,7 +3352,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-07-30T16:09:03.169409</t>
+          <t>2025-07-30T16:29:42.353424</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3352,128 +3377,6 @@
         </is>
       </c>
       <c r="H47" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    fibonacci_list = [0, 1]
-    for i in range(2, n):
-        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
-    return fibonacci_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    fibonacci_list = [0, 1]
-    for i in range(2, n):
-        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
-    return fibonacci_list[:n]
-```</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>fibonacci-2</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:09:04.131325</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
-        <v>2</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    result = []
-    a, b = 0, 1
-    for _ in range(n):
-        result.append(a)
-        a, b = b, a + b
-    return result
-```</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>```python
-def fibonacci(n):
-    result = []
-    a, b = 0, 1
-    for _ in range(n):
-        result.append(a)
-        a, b = b, a + b
-    return result
-```</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>fibonacci-3</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:09:05.134661</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>3</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
@@ -3484,7 +3387,7 @@
 ```</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>```python
 def fibonacci(n):
@@ -3495,6 +3398,124 @@
 ```</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>fibonacci-2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:43.348027</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    sequence = [0, 1]
+    while len(sequence) &lt; n:
+        sequence.append(sequence[-1] + sequence[-2])
+    return sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    sequence = [0, 1]
+    while len(sequence) &lt; n:
+        sequence.append(sequence[-1] + sequence[-2])
+    return sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>fibonacci-3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:29:45.073206</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    for i in range(2, n):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -3508,7 +3529,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-07-30T16:09:06.585064</t>
+          <t>2025-07-30T16:29:46.387728</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3567,7 +3588,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-07-30T16:09:07.803538</t>
+          <t>2025-07-30T16:29:47.728570</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3596,8 +3617,8 @@
           <t>```python
 def fibonacci(n):
     fib_list = [0, 1]
-    for i in range(2, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
     return fib_list[:n]
 ```</t>
         </is>
@@ -3607,8 +3628,8 @@
           <t>```python
 def fibonacci(n):
     fib_list = [0, 1]
-    for i in range(2, n):
-        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
     return fib_list[:n]
 ```</t>
         </is>

</xml_diff>

<commit_message>
running tests temp 0.5
</commit_message>
<xml_diff>
--- a/outputs/results.xlsx
+++ b/outputs/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3639,6 +3639,1552 @@
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>fibonacci_2-1</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:12.123258</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>fibonacci_2-2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:14.787462</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>fibonacci_2-3</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:16.678953</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>3</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib_list = fibonacci_2(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>fibonacci_2-4</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:18.086108</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>4</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>fibonacci_2-5</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:20.971650</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_2' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>5</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>4552c0cc3820a4022c435202f1af1a231866f6c9d8e10f818b03e13eb57f42de</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib
+```</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>def fibonacci_2(n):
+    if n &lt;= 0:
+        return []
+    elif n == 1:
+        return [0]
+    elif n == 2:
+        return [0, 1]
+    else:
+        fib = fibonacci_2(n - 1)
+        fib.append(fib[-1] + fib[-2])
+        return fib</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>fibonacci_3-1</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:21.936419</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>fibonacci_3-2</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:23.245017</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>2</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2] + fib_list[-3])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib_list = [0, 1, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2] + fib_list[-3])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>fibonacci_3-3</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:24.173110</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>3</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib_list = [0, 1]
+    for i in range(1, 2):
+        fib_list.append(fib_list[i] + fib_list[i-1])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib_list = [0, 1]
+    for i in range(1, 2):
+        fib_list.append(fib_list[i] + fib_list[i-1])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>fibonacci_3-4</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:25.826875</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>4</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib = [0, 1]
+    for i in range(1, 3):
+        fib.append(fib[i] + fib[i-1])
+    return fib
+```</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3():
+    fib = [0, 1]
+    for i in range(1, 3):
+        fib.append(fib[i] + fib[i-1])
+    return fib
+```</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>fibonacci_3-5</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:26.906908</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_3' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>5</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>35aed33e90be392997a6c3bb0c705d9697648fbcba99206bdc24e2415febc3eb</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib = [0, 1, 1]
+    for i in range(3, n):
+        fib.append(fib[i-1] + fib[i-2] + fib[i-3])
+    return fib[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_3(n):
+    fib = [0, 1, 1]
+    for i in range(3, n):
+        fib.append(fib[i-1] + fib[i-2] + fib[i-3])
+    return fib[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>fibonacci_4-1</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:28.135485</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fibonacci_list = [0, 1]
+    for i in range(2, 4):
+        fibonacci_list.append(fibonacci_list[i-1] + fibonacci_list[i-2])
+    return fibonacci_list
+```</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>fibonacci_4-2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:29.252422</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>2</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>fibonacci_4-3</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:30.161929</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>3</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>fibonacci_4-4</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:31.105712</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>4</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>fibonacci_4-5</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:32.250381</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_4' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>5</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>b6b6109cc2f0995443320ecd4fc852e5ff57c6f08c3a0dcaf9d6c6f028bcbf07</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_4():
+    fib_list = [0, 1]
+    for i in range(2, 4):
+        fib_list.append(fib_list[i-1] + fib_list[i-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>fibonacci_5-1</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:33.285911</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]
+```</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]
+</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>fibonacci_5-2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:34.470317</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return [0] if n == 0 else [0, 1]
+    else:
+        fib_list = fibonacci_5(n - 1)
+        fib_list.append(fib_list[-1] + fib_list[-2])
+        return fib_list
+print(fibonacci_5(5))
+```</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>fibonacci_5-3</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:36.204454</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>3</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]
+```</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>fibonacci_5-4</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:38.121215</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>4</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    result = []
+    for i in range(5):
+        result.append(fibonacci_5(i))
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    result = []
+    for i in range(5):
+        result.append(fibonacci_5(i))
+    return result
+```</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>fibonacci_5-5</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:39.126211</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci_5' that returns a list. Use recursion. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>5</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>5ab6c8f7aa6038d70f5b38c68fcbf0ff8f365af9691a5383669645592c9a0988</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5_list():
+    return [fibonacci_5(i) for i in range(5)]
+```</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>def fibonacci_5(n):
+    if n &lt;= 1:
+        return n
+    else:
+        return fibonacci_5(n-1) + fibonacci_5(n-2)
+def fibonacci_5():
+    return [fibonacci_5(i) for i in range(5)]</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>fibonacci-1</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:40.511802</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>fibonacci-2</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:42.693655</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>fibonacci-3</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:43.625137</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>3</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>fibonacci-4</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:45.331013</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>4</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_sequence = [0, 1]
+    for i in range(2, n):
+        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2])
+    return fib_sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_sequence = [0, 1]
+    for i in range(2, n):
+        fib_sequence.append(fib_sequence[i-1] + fib_sequence[i-2])
+    return fib_sequence[:n]
+```</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>fibonacci-5</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2025-07-30T16:32:46.723378</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Write a python function named 'fibonacci' that returns a list. Do not include comments. Output only the code.</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>5</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>5e03e399ca7dc2452534428b7f54079e047f57cb28da36bcd17cd19a71a4257b</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>```python
+def fibonacci(n):
+    fib_list = [0, 1]
+    while len(fib_list) &lt; n:
+        fib_list.append(fib_list[-1] + fib_list[-2])
+    return fib_list
+```</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>